<commit_message>
new data + meeting minutes
</commit_message>
<xml_diff>
--- a/data/input/eurobank/202509.xlsx
+++ b/data/input/eurobank/202509.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cervedgroup-my.sharepoint.com/personal/alexis_milionis_cerved_com/Documents/codebase/Utilities/streamlit/data/input/eurobank/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="68" documentId="11_F235BD1891344565E00B8F3D5E94DAA62ED55A21" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8B7FA506-8F09-4DE2-B345-2ADB3D82106F}"/>
+  <xr:revisionPtr revIDLastSave="74" documentId="11_F235BD1891344565E00B8F3D5E94DAA62ED55A21" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B1D254AA-4C82-4328-8E87-4D6B6762E42B}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1125" yWindow="1125" windowWidth="17280" windowHeight="8925" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Φύλλο1" sheetId="1" r:id="rId1"/>
@@ -3357,9 +3357,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:AQ489"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A387" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J488" sqref="J488"/>
+      <selection pane="bottomLeft" activeCell="W9" sqref="W9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -41567,9 +41567,64 @@
   </sheetData>
   <autoFilter ref="A1:AQ481" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <filterColumn colId="8">
-      <customFilters>
-        <customFilter operator="notEqual" val="*eurobank*"/>
-      </customFilters>
+      <filters>
+        <filter val="SOUTHROCK PROPERTY COMPANY ONE A.E."/>
+        <filter val="ΑΓΓΕΛΟΠΟΥΛΟΣ ΠΑΥΛΟΣ"/>
+        <filter val="ΑΚΑΔΗΜΙΑ ΑΘΗΝΩΝ ΕΓΓΟΝΟΠΟΥΛΟΣ Κ00"/>
+        <filter val="ΑΝΑΓΝΩΣΤΟΠΟΥΛΟΣ ΑΘΑΝ, ΝΙΚ ΚΛΠ"/>
+        <filter val="ΑΠΟΣΤΟΛΟΥ ΝΕΣΤΩΡ ΚΛΠ ΣΥΝΙΔ"/>
+        <filter val="ΑΥΣΤΡΙΑΚΕΣ ΑΕΡΟΠΟΡΙΚΕΣ ΓΡΑΜΜΕΣ00"/>
+        <filter val="ΑΦΟΙ ΚΑΡΑΤΖΑ Α.Ε."/>
+        <filter val="ΒΑΣΙΛΟΠΟΥΛΟΣ ΙΩΑΝΝΗΣ"/>
+        <filter val="ΒΕΝΕΤΣΑΝΟΣ ΠΕΤΡΟΣ"/>
+        <filter val="ΒΛΑΧΟΥΛΗ-ΚΑΡΕΛΑ ΧΡΙΣΤΙΝΑ"/>
+        <filter val="ΒΟΡΡΕΑΣ ΠΑΝΤΕΛΗΣ"/>
+        <filter val="ΒΟΥΛΓΟΥΡΙΔΗ ΠΑΡΑΣΚΕΥΗ"/>
+        <filter val="Γ  ΝΟΙΚΟΚΥΡΑΚΗ ΚΑΙ ΣΙΑ ΟΕ"/>
+        <filter val="ΓΑΒΑΛΑΚΗ ΕΥΓΕΝΙΑ ΚΛΠ ΣΥΝΙΔΙΟΚΤ."/>
+        <filter val="ΓΕΩΡΓΑΚΗΣ ΔΗΜΟΣΘ &amp; ΛΟΙΠΟΙ ΣΥΝΙΔ"/>
+        <filter val="ΓΚΑΤΖΩΝΗΣ ΑΝΤΩΝΗΣ ΚΛΠ ΣΥΝΙΔ"/>
+        <filter val="ΔΑΒΒΕΤΑ ΓΕΩΡΓΙΑ ΚΛΠ"/>
+        <filter val="ΔΗΜΙΟΥΡΓΙΑ ΑΝ ΚΤΗΜ ΤΕΧΝ ΕΤΑΙ  00"/>
+        <filter val="Ε. ΣΠΑΘΑΡΙΩΤΗ ΑΕ"/>
+        <filter val="ΕΘΝΙΚΟΝ ΙΔΡΥΜΑ ΕΡΕΥΝΩΝ        00"/>
+        <filter val="ΕΛΥΡΟΣ Α.Ε."/>
+        <filter val="ΙΔΡΥΜΑ ΕΥΓΕΝΙΔΟΥ              00"/>
+        <filter val="ΙΩΣΗΦ ΓΟΥΜΕΝΑΚΗΣ &amp; ΣΙΑ Ε.Ε."/>
+        <filter val="ΚΑΛΥΨΩ ΑΕΒΕ                   00"/>
+        <filter val="ΚΑΡΝΑΧΩΡΙΤΗ ΑΝΝΑ"/>
+        <filter val="ΚΟΝΣΟΥΛΑΣ ΙΩΑΝΝΗΣ             00"/>
+        <filter val="ΚΟΝΣΟΥΛΑΣ ΠΑΝΑΓΙΩΤΗΣ Ε.Π.Ε"/>
+        <filter val="ΚΟΥΤΣΟΓΙΑΝΝΗΣ ΔΙΟΝΥΣΙΟΣ ΤΟΥ ΛΕΩΝ"/>
+        <filter val="ΚΥΡΙΑΚΙΔΗΣ ΣΩΤΗΡΙΟΣ &amp; ΛΟΙΠΟΙ ΣΥΝ"/>
+        <filter val="ΛΙΒΑ ΓΕΩΡΓΟΥΝΤΖΟΥ ΑΙΚΑΤΕΡΙΝΗ"/>
+        <filter val="ΛΟΓΟΘΕΤΗΣ ΗΡΑΚΛΗΣ &amp; ΛΟΙΠΟΙ ΣΥΝΙΔ"/>
+        <filter val="ΛΟΓΟΘΕΤΗΣ ΝΙΚ ΗΡΑΚΛ ΜΕΣΣΗΝΗΣ Θ Α"/>
+        <filter val="ΛΟΥΠΑΣΑΚΗΣ-ΛΟΥΠΑΣΗΣ ΠΑΝΑΓΙΩΤΗΣ"/>
+        <filter val="ΜΑΝΤΖΑΡΗΣ ΔΗΜΗΤΡΙΟΣ"/>
+        <filter val="ΜΑΝΤΖΟΥΡΙΔΗΣ ΣΩΤΗΡΙΟΣ"/>
+        <filter val="ΜΕΤΟΧ ΤΑΜΕΙΟ ΠΟΛΙΤΙΚΩΝ ΥΠΑΛΛΗΛΩΝ"/>
+        <filter val="ΜΠΑΡΑΜΠΟΥΤΗΣ ΚΩΝΣΤΑΝΤΙΝΟΣ"/>
+        <filter val="ΜΠΟΤΣΑΡΗ ΠΗΝΕΛΟΠΗ ΕΛΕΝΗ"/>
+        <filter val="ΜΥΛΩΝΑΣ ΙΩΑΝΝΗΣ &amp; ΛΟΙΠΟΙ ΣΥΝΙΔ"/>
+        <filter val="ΝΕΟΦΩΤΙΣΤΟΣ ΔΗΜ. &amp; ΠΑΝΩΡΑΙΑ"/>
+        <filter val="ΞΥΔΙΑΣ ΔΗΜΗΤΡΙΟΣ &amp; ΛΟΙΠΟΙ ΣΥΝ"/>
+        <filter val="ΟΥΡΑΝΗ ΕΛΕΝΗ                  00"/>
+        <filter val="ΠΡΩΤΟΓΕΡΟΣ ΘΩΜΑΣ"/>
+        <filter val="ΡΟΥΣΣΟΥ ΑΝ &amp; ΠΑΠΑΘΑΝΑΣΙΟΥ ΜΑΡΙΑ"/>
+        <filter val="ΣΑΣΣΑΛΟΥ ΣΟΦΙΑ"/>
+        <filter val="ΣΑΣΣΑΛΟΥ ΣΟΦΙΑ &amp; ΛΟΙΠΟΙ ΣΥΝΙΔ"/>
+        <filter val="ΣΕΚΟΠΟΥΛΟΥ ΙΩΣΗΦΙΝΑ"/>
+        <filter val="ΣΙΔΕΡΗΣ ΔΗΜΗΤΡΙΟΣ &amp; ΣΙΑ ΑΕ"/>
+        <filter val="ΣΚΑΦΙΔΑΚΗΣ ΝΙΚ &amp; ΛΟΙΠΟΙ ΣΥΝΙΔ"/>
+        <filter val="ΣΠΑΘΑΚΗΣ-ΝΙΩΡΑΣ- ΓΙΑΤΡΑ ΟΕ"/>
+        <filter val="ΣΤΕΦΑΝΟΥ ΓΕΩΡΓ"/>
+        <filter val="ΤΡΟΥΠΑΚΗΣ ΘΕΟΦΑΝΗΣ"/>
+        <filter val="ΤΣΑΚΙΡΗ ΧΡΙΣΤΙΝΑ"/>
+        <filter val="ΤΣΑΜΠΑΡΛΙΔΗΣ ΓΕΩΡΓΙΟΣ ΚΛΠ"/>
+        <filter val="ΤΣΙΓΚΟΣ ΔΗΜΗΤΡΗΣ &amp; ΙΣΙΔΩΡΟΣ"/>
+        <filter val="ΤΣΟΥΜΑΣ ΠΕΤΡΟΣ ΚΛΠ ΣΥΝΙΔ"/>
+      </filters>
     </filterColumn>
     <filterColumn colId="9">
       <filters>

</xml_diff>